<commit_message>
Kosten bei 9_1 je Teilvariante
auswertung auch etwas geändert sodass 20 drin ist
Simulation auch angelegt für 20
</commit_message>
<xml_diff>
--- a/9_1_Kosten/9_2_Kosten_10.xlsx
+++ b/9_1_Kosten/9_2_Kosten_10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fraunhofer-my.sharepoint.com/personal/lara_josephine_barnic_iee_fraunhofer_de/Documents/A_Bearbeitung/9_Parameterstudie_REP/9_1_Kosten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1588" documentId="11_AD4DB114E441178AC67DF4879E90C19A693EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40190341-B63F-469F-A8C4-8EFD072D4FEA}"/>
+  <xr:revisionPtr revIDLastSave="1626" documentId="11_AD4DB114E441178AC67DF4879E90C19A693EDF21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E57FA2C9-EBC1-41CC-8D38-FA88B9082EFB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zusammenfassung" sheetId="8" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Kostenposten_8.2.2" sheetId="9" r:id="rId3"/>
     <sheet name="dezentral" sheetId="1" r:id="rId4"/>
     <sheet name="kalte NW" sheetId="7" r:id="rId5"/>
-    <sheet name="NT-WN_3_77" sheetId="6" r:id="rId6"/>
+    <sheet name="NT-WN_10" sheetId="6" r:id="rId6"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="128">
   <si>
     <t>Investitionskosten</t>
   </si>
@@ -448,6 +448,9 @@
   </si>
   <si>
     <t>WW-WP Abwärme</t>
+  </si>
+  <si>
+    <t>Netzstrombedarfe</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -536,6 +539,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="10">
@@ -881,7 +890,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -995,6 +1004,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1093,7 +1103,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{058AF01F-20EA-4922-B236-FFBBD3D75E79}" type="CELLRANGE">
+                    <a:fld id="{B0208CC4-FA0A-43C6-BEEC-24C5374B5B08}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1126,7 +1136,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6FDA785C-5F10-49E9-9C74-2176A3F94FB3}" type="CELLRANGE">
+                    <a:fld id="{35CA1B61-0720-45B2-A8B4-06718C468A7B}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1160,7 +1170,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BAAF923F-7535-44AB-B862-92A1A61A5272}" type="CELLRANGE">
+                    <a:fld id="{490393E5-7943-4AC2-B24A-0715E4A1FA09}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1239,7 +1249,7 @@
                   <c:v>2.0695804917797993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8028352280134901</c:v>
+                  <c:v>1.7569054221193687</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.1404929913135451</c:v>
@@ -1674,7 +1684,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D2D5CCB-B740-4BDE-BE9E-9EDA474A63EB}" type="CELLRANGE">
+                    <a:fld id="{1528952F-DA0D-462E-B317-678C35BDF745}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1708,7 +1718,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52AF3E92-FF4C-4E7D-B390-36B95EA844A6}" type="CELLRANGE">
+                    <a:fld id="{2F3C0039-ADF0-4A69-A6A0-E1788B615C8B}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -1787,7 +1797,7 @@
                   <c:v>2.0695804917797993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8028352280134901</c:v>
+                  <c:v>1.7569054221193687</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.1404929913135451</c:v>
@@ -2462,7 +2472,7 @@
                   <c:v>167566.24131354483</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>576996.74237317289</c:v>
+                  <c:v>531066.93647905171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2832,7 +2842,7 @@
                   <c:v>0.73814771008916502</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34944957265683402</c:v>
+                  <c:v>0.35858503939274433</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2897,7 +2907,7 @@
                   <c:v>3.8003488135731164E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16425665587121607</c:v>
+                  <c:v>0.16855072669938947</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2962,7 +2972,7 @@
                   <c:v>0.11387283256200852</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14839725552445113</c:v>
+                  <c:v>0.15227672282852281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3027,7 +3037,7 @@
                   <c:v>7.8283947666988332E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.32004962705823908</c:v>
+                  <c:v>0.30227406085321401</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3092,7 +3102,7 @@
                   <c:v>3.1692021546107056E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7846888889259737E-2</c:v>
+                  <c:v>1.8313450226129444E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5677,9 +5687,6 @@
           <cell r="C4">
             <v>49237.671936835155</v>
           </cell>
-          <cell r="D4">
-            <v>149735.09182771994</v>
-          </cell>
           <cell r="E4">
             <v>41164.404932023172</v>
           </cell>
@@ -5732,6 +5739,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5999,8 +6010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5395E545-C7E4-4937-89EC-C03939104281}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6036,7 +6047,7 @@
       </c>
       <c r="C2" s="47">
         <f t="shared" ref="C2:D2" si="0">C5/1000000</f>
-        <v>1.8028352280134901</v>
+        <v>1.7569054221193687</v>
       </c>
       <c r="D2" s="42">
         <f t="shared" si="0"/>
@@ -6086,11 +6097,11 @@
       </c>
       <c r="M3" s="3">
         <f>(K3-K4)/K4</f>
-        <v>0.14795875941487499</v>
+        <v>0.17796920979573744</v>
       </c>
       <c r="N3" s="3">
         <f>K3-K4</f>
-        <v>0.26674526376630925</v>
+        <v>0.31267506966043057</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -6102,7 +6113,7 @@
       </c>
       <c r="K4" s="42">
         <f>C2</f>
-        <v>1.8028352280134901</v>
+        <v>1.7569054221193687</v>
       </c>
       <c r="L4" s="42">
         <v>557.10423600000001</v>
@@ -6114,8 +6125,8 @@
         <v>2069580.4917797993</v>
       </c>
       <c r="C5" s="42">
-        <f>'NT-WN_3_77'!B29</f>
-        <v>1802835.2280134901</v>
+        <f>'NT-WN_10'!B29</f>
+        <v>1756905.4221193688</v>
       </c>
       <c r="D5" s="42">
         <f>'kalte NW'!B30</f>
@@ -6133,19 +6144,19 @@
       </c>
       <c r="M5" s="3">
         <f>(K5-K4)/K4</f>
-        <v>0.18729263664994705</v>
+        <v>0.21833137080962028</v>
       </c>
       <c r="N5" s="3">
         <f>K5-K4</f>
-        <v>0.33765776330005504</v>
+        <v>0.38358756919417636</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="74" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -6153,31 +6164,31 @@
       </c>
       <c r="B7" s="3">
         <f>B5-C5</f>
-        <v>266745.26376630925</v>
+        <v>312675.06966043054</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="3">
         <f>D5-C5</f>
-        <v>337657.76330005494</v>
+        <v>383587.56919417623</v>
       </c>
       <c r="F7" s="3">
         <f>D2-C2</f>
-        <v>0.33765776330005504</v>
+        <v>0.38358756919417636</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B8" s="45">
         <f>B7/C5</f>
-        <v>0.14795875941487496</v>
+        <v>0.17796920979573741</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="45">
         <f>D7/C5</f>
-        <v>0.187292636649947</v>
+        <v>0.2183313708096202</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3">
@@ -6186,11 +6197,11 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
@@ -6220,12 +6231,12 @@
       <c r="E11" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -6255,7 +6266,7 @@
       </c>
       <c r="C15">
         <f>C2/C14</f>
-        <v>5.9521204045418917E-4</v>
+        <v>5.8004816243632502E-4</v>
       </c>
       <c r="D15">
         <f>D2/D14</f>
@@ -6278,7 +6289,7 @@
   <dimension ref="B1:M46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6286,6 +6297,7 @@
     <col min="3" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.7265625" customWidth="1"/>
     <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.453125" customWidth="1"/>
@@ -6296,6 +6308,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>127</v>
+      </c>
+    </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>13</v>
@@ -6306,6 +6323,13 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
+      <c r="G3">
+        <v>2.5</v>
+      </c>
+      <c r="H3" s="3">
+        <v>146736.91835603901</v>
+      </c>
+      <c r="I3" s="73"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -6314,11 +6338,32 @@
       <c r="C4" t="s">
         <v>83</v>
       </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3">
+        <v>144131.19078266801</v>
+      </c>
+      <c r="I4" s="73"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>7.5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>141702.40077180401</v>
+      </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3">
+        <v>139266.76</v>
+      </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
@@ -6330,6 +6375,12 @@
       <c r="E7" t="s">
         <v>49</v>
       </c>
+      <c r="G7">
+        <v>12.5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>136824.21837352001</v>
+      </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
@@ -6340,7 +6391,7 @@
         <v>289881.59328429529</v>
       </c>
       <c r="D8" s="2">
-        <v>656962.71539412113</v>
+        <v>611032.90949999995</v>
       </c>
       <c r="E8" s="2">
         <v>257330.43434875214</v>
@@ -6378,11 +6429,11 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D13" s="74" t="s">
+      <c r="D13" s="75" t="s">
         <v>123</v>
       </c>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
       <c r="I13" t="s">
         <v>55</v>
       </c>
@@ -6396,8 +6447,8 @@
         <v>66069.878811235394</v>
       </c>
       <c r="E14" s="38">
-        <f>[1]Netzstrom_PV_Strom!$D$4</f>
-        <v>149735.09182771994</v>
+        <f>H6</f>
+        <v>139266.76</v>
       </c>
       <c r="F14" s="38">
         <f>[1]Netzstrom_PV_Strom!$F$4</f>
@@ -6472,7 +6523,7 @@
       </c>
       <c r="E17" s="3">
         <f>$C17*$E$14/100</f>
-        <v>34004.8393540752</v>
+        <v>31627.481196000004</v>
       </c>
       <c r="F17" s="3">
         <f>$C17*$F$14/100</f>
@@ -6514,7 +6565,7 @@
       </c>
       <c r="E18" s="3">
         <f t="shared" ref="E18:E38" si="2">$C18*$E$14/100</f>
-        <v>31998.389123583751</v>
+        <v>29761.306612000004</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" ref="F18:F38" si="3">$C18*$F$14/100</f>
@@ -6556,7 +6607,7 @@
       </c>
       <c r="E19" s="3">
         <f t="shared" si="2"/>
-        <v>30740.614352230903</v>
+        <v>28591.465828000004</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="3"/>
@@ -6598,7 +6649,7 @@
       </c>
       <c r="E20" s="3">
         <f t="shared" si="2"/>
-        <v>30231.51504001666</v>
+        <v>28117.958844000004</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="3"/>
@@ -6640,7 +6691,7 @@
       </c>
       <c r="E21" s="3">
         <f t="shared" si="2"/>
-        <v>30141.673984920024</v>
+        <v>28034.398788000002</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="3"/>
@@ -6682,7 +6733,7 @@
       </c>
       <c r="E22" s="3">
         <f t="shared" si="2"/>
-        <v>30276.435567564968</v>
+        <v>28159.738872000002</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="3"/>
@@ -6725,7 +6776,7 @@
       </c>
       <c r="E23" s="3">
         <f t="shared" si="2"/>
-        <v>30246.488549199425</v>
+        <v>28131.88552</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="3"/>
@@ -6768,7 +6819,7 @@
       </c>
       <c r="E24" s="3">
         <f t="shared" si="2"/>
-        <v>30216.541530833882</v>
+        <v>28104.032168000002</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="3"/>
@@ -6811,7 +6862,7 @@
       </c>
       <c r="E25" s="3">
         <f t="shared" si="2"/>
-        <v>30186.594512468339</v>
+        <v>28076.178816000003</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="3"/>
@@ -6854,7 +6905,7 @@
       </c>
       <c r="E26" s="3">
         <f t="shared" si="2"/>
-        <v>30156.647494102795</v>
+        <v>28048.325464000005</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="3"/>
@@ -6896,7 +6947,7 @@
       </c>
       <c r="E27" s="3">
         <f t="shared" si="2"/>
-        <v>30126.700475737252</v>
+        <v>28020.472112000003</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="3"/>
@@ -6942,7 +6993,7 @@
       </c>
       <c r="E28" s="3">
         <f t="shared" si="2"/>
-        <v>29821.240888408702</v>
+        <v>27736.367921600002</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="3"/>
@@ -6985,7 +7036,7 @@
       </c>
       <c r="E29" s="3">
         <f t="shared" si="2"/>
-        <v>29515.781301080155</v>
+        <v>27452.263731200001</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="3"/>
@@ -7028,7 +7079,7 @@
       </c>
       <c r="E30" s="3">
         <f t="shared" si="2"/>
-        <v>29210.321713751604</v>
+        <v>27168.159540799999</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="3"/>
@@ -7071,7 +7122,7 @@
       </c>
       <c r="E31" s="3">
         <f t="shared" si="2"/>
-        <v>28904.862126423057</v>
+        <v>26884.055350399998</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="3"/>
@@ -7113,7 +7164,7 @@
       </c>
       <c r="E32" s="3">
         <f t="shared" si="2"/>
-        <v>28599.40253909451</v>
+        <v>26599.951160000004</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="3"/>
@@ -7155,7 +7206,7 @@
       </c>
       <c r="E33" s="3">
         <f t="shared" si="2"/>
-        <v>28779.084649287768</v>
+        <v>26767.071272000001</v>
       </c>
       <c r="F33" s="3">
         <f t="shared" si="3"/>
@@ -7198,7 +7249,7 @@
       </c>
       <c r="E34" s="3">
         <f t="shared" si="2"/>
-        <v>28773.095245614662</v>
+        <v>26761.500601599997</v>
       </c>
       <c r="F34" s="3">
         <f t="shared" si="3"/>
@@ -7241,7 +7292,7 @@
       </c>
       <c r="E35" s="3">
         <f t="shared" si="2"/>
-        <v>28767.105841941549</v>
+        <v>26755.929931199997</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="3"/>
@@ -7284,7 +7335,7 @@
       </c>
       <c r="E36" s="3">
         <f t="shared" si="2"/>
-        <v>28761.116438268436</v>
+        <v>26750.359260799996</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="3"/>
@@ -7327,7 +7378,7 @@
       </c>
       <c r="E37" s="3">
         <f t="shared" si="2"/>
-        <v>28755.127034595331</v>
+        <v>26744.788590399992</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="3"/>
@@ -7369,7 +7420,7 @@
       </c>
       <c r="E38" s="3">
         <f t="shared" si="2"/>
-        <v>28749.137630922225</v>
+        <v>26739.217919999999</v>
       </c>
       <c r="F38" s="3">
         <f t="shared" si="3"/>
@@ -7408,7 +7459,7 @@
       </c>
       <c r="E40" s="3">
         <f>SUM(E17:E38)</f>
-        <v>656962.71539412113</v>
+        <v>611032.90949999995</v>
       </c>
       <c r="F40" s="3">
         <f>SUM(F17:F38)</f>
@@ -7448,20 +7499,20 @@
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B42" s="75" t="s">
+      <c r="B42" s="76" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="75"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="75"/>
-      <c r="F42" s="75"/>
-      <c r="G42" s="75"/>
-      <c r="H42" s="75"/>
-      <c r="I42" s="75"/>
-      <c r="J42" s="75"/>
-      <c r="K42" s="75"/>
-      <c r="L42" s="75"/>
-      <c r="M42" s="75"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="76"/>
+      <c r="H42" s="76"/>
+      <c r="I42" s="76"/>
+      <c r="J42" s="76"/>
+      <c r="K42" s="76"/>
+      <c r="L42" s="76"/>
+      <c r="M42" s="76"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B43" s="40">
@@ -7476,7 +7527,7 @@
       </c>
       <c r="E43" s="41">
         <f>$C43*$E$14/100</f>
-        <v>38826.309310927776</v>
+        <v>36111.870867999998</v>
       </c>
       <c r="F43" s="41">
         <f>$C43*$D$14/100</f>
@@ -7519,7 +7570,7 @@
       </c>
       <c r="E44" s="41">
         <f>$C44*$E$14/100</f>
-        <v>40608.156903677649</v>
+        <v>37769.145312000008</v>
       </c>
       <c r="F44" s="41">
         <f>$C44*$D$14/100</f>
@@ -7562,7 +7613,7 @@
       </c>
       <c r="E45" s="41">
         <f>$C45*$E$14/100</f>
-        <v>36580.282933511982</v>
+        <v>34022.869467999997</v>
       </c>
       <c r="F45" s="41">
         <f>$C45*$D$14/100</f>
@@ -7605,7 +7656,7 @@
       </c>
       <c r="E46" s="41">
         <f>$C46*$E$14/100</f>
-        <v>36864.779607984652</v>
+        <v>34287.476311999999</v>
       </c>
       <c r="F46" s="41">
         <f>$C46*$D$14/100</f>
@@ -7681,7 +7732,7 @@
         <v>KNW</v>
       </c>
       <c r="D2" s="42" t="str" cm="1">
-        <f t="array" ref="D2:D9">'NT-WN_3_77'!C32:C39</f>
+        <f t="array" ref="D2:D9">'NT-WN_10'!C32:C39</f>
         <v>NT-WN</v>
       </c>
       <c r="G2" s="42" t="s">
@@ -7728,7 +7779,7 @@
       </c>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
-        <v>0.34944957265683402</v>
+        <v>0.35858503939274433</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -7761,7 +7812,7 @@
       </c>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
-        <v>0.16425665587121607</v>
+        <v>0.16855072669938947</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -7794,7 +7845,7 @@
       </c>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
-        <v>0.14839725552445113</v>
+        <v>0.15227672282852281</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -7808,7 +7859,7 @@
         <v>167566.24131354483</v>
       </c>
       <c r="D6" s="2">
-        <v>576996.74237317289</v>
+        <v>531066.93647905171</v>
       </c>
       <c r="E6" s="2"/>
       <c r="G6" s="2">
@@ -7827,7 +7878,7 @@
       </c>
       <c r="K6" s="2">
         <f t="shared" si="0"/>
-        <v>0.32004962705823908</v>
+        <v>0.30227406085321401</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -7860,7 +7911,7 @@
       </c>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
-        <v>1.7846888889259737E-2</v>
+        <v>1.8313450226129444E-2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -7886,7 +7937,7 @@
         <v>2140492.9913135446</v>
       </c>
       <c r="D9" s="2">
-        <v>1802835.2280134901</v>
+        <v>1756905.4221193688</v>
       </c>
       <c r="E9" s="2"/>
       <c r="H9" t="s">
@@ -7902,7 +7953,7 @@
       </c>
       <c r="K9" s="42">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -7932,7 +7983,7 @@
       </c>
       <c r="C12" s="46">
         <f>ROUND(D9,-4)</f>
-        <v>1800000</v>
+        <v>1760000</v>
       </c>
       <c r="D12" s="46">
         <f>ROUND(C9,-4)</f>
@@ -8060,7 +8111,7 @@
         <v>167566.24131354483</v>
       </c>
       <c r="E38" s="2">
-        <v>576996.74237317289</v>
+        <v>531066.93647905171</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
@@ -8134,21 +8185,21 @@
       <c r="A1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="76" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="79"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="21" t="s">
@@ -8682,21 +8733,21 @@
       <c r="A1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="76" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="79"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="21" t="s">
@@ -9362,8 +9413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B9FB241-9669-439D-99A8-3E2AD756299A}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9384,21 +9435,21 @@
       <c r="A1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="76" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="79"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="21" t="s">
@@ -9471,7 +9522,7 @@
       </c>
       <c r="L5" s="7" cm="1">
         <f t="array" ref="L5:L6">'Allgemeine Parameter'!D8:D9</f>
-        <v>656962.71539412113</v>
+        <v>611032.90949999995</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
@@ -9862,7 +9913,7 @@
       <c r="A29" s="28"/>
       <c r="B29" s="33">
         <f>SUM(C29,I29,L29)</f>
-        <v>1802835.2280134901</v>
+        <v>1756905.4221193688</v>
       </c>
       <c r="C29" s="17">
         <f>SUM(C1:C26)</f>
@@ -9875,7 +9926,7 @@
       </c>
       <c r="L29" s="54">
         <f>SUM(L5:L6)</f>
-        <v>576996.74237317289</v>
+        <v>531066.93647905171</v>
       </c>
       <c r="M29"/>
       <c r="N29"/>
@@ -9902,7 +9953,7 @@
         <f>'kalte NW'!L30</f>
         <v>167566.24131354483</v>
       </c>
-      <c r="M31" s="79" t="s">
+      <c r="M31" s="80" t="s">
         <v>119</v>
       </c>
     </row>
@@ -9918,9 +9969,9 @@
       <c r="K32"/>
       <c r="L32" s="3">
         <f>L29-L31</f>
-        <v>409430.50105962809</v>
-      </c>
-      <c r="M32" s="79"/>
+        <v>363500.69516550691</v>
+      </c>
+      <c r="M32" s="80"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B33" s="60" t="s">
@@ -9934,9 +9985,9 @@
       <c r="K33"/>
       <c r="L33" s="3">
         <f>L32/25</f>
-        <v>16377.220042385125</v>
-      </c>
-      <c r="M33" s="79"/>
+        <v>14540.027806620277</v>
+      </c>
+      <c r="M33" s="80"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B34" s="49" t="s">
@@ -9968,7 +10019,7 @@
       </c>
       <c r="C36" s="67">
         <f>SUM(L29)</f>
-        <v>576996.74237317289</v>
+        <v>531066.93647905171</v>
       </c>
       <c r="I36"/>
       <c r="K36"/>
@@ -10000,7 +10051,7 @@
       </c>
       <c r="C39" s="33">
         <f>SUM(C33:C37)</f>
-        <v>1802835.2280134901</v>
+        <v>1756905.4221193688</v>
       </c>
       <c r="I39"/>
       <c r="K39"/>

</xml_diff>